<commit_message>
buat folder mahasiswa, dosen, admin
</commit_message>
<xml_diff>
--- a/chtGPT.xlsx
+++ b/chtGPT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Android\Android\elearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7F8897-E0B3-4970-8B96-4898F57C3DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411420EE-1F99-417B-8B77-08AC57C23725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1F536944-2D82-4B74-8666-560C579C7821}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="15375" windowHeight="7875" xr2:uid="{1F536944-2D82-4B74-8666-560C579C7821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>module</t>
   </si>
@@ -53,7 +53,13 @@
     <t>taskTab</t>
   </si>
   <si>
-    <t xml:space="preserve">makasihbanyak7@gmail.com, </t>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Snack Bar (berhasil/gagal)</t>
+  </si>
+  <si>
+    <t>makasihbanyak7@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -110,18 +116,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -457,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59D498C-6602-42D3-89A9-88C3A99F959E}">
-  <dimension ref="A6:C14"/>
+  <dimension ref="A6:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,68 +523,82 @@
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A10"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{F9B9EB14-A285-413A-9C5C-375A3F4A4616}"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{F9B9EB14-A285-413A-9C5C-375A3F4A4616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>